<commit_message>
Fixed issue due to mis-configured regfile
Both the data was not updated, and the file path was wrong
</commit_message>
<xml_diff>
--- a/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
+++ b/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese_ford1\Documents\GitHub\ARM-Lab\ARM-Lab\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese\Documents\GitHub\ARM-Lab\ARM-Lab\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD7C078-8BBC-4953-AB5D-63FFCBFCA3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C979CB96-A95A-4F73-8C3A-EC31AA7F08A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -328,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -336,7 +336,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +619,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,28 +1273,28 @@
       <c r="C20" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="D20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1306,25 +1305,25 @@
       <c r="D21" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="E21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Various Fixing of iDecode Er Values
And other things
</commit_message>
<xml_diff>
--- a/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
+++ b/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese\Documents\GitHub\ARM-Lab\ARM-Lab\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C979CB96-A95A-4F73-8C3A-EC31AA7F08A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383A21BD-D543-4E7E-B0EE-311AF023E8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="76">
   <si>
     <t>Instruction 1</t>
   </si>
@@ -144,12 +144,6 @@
     <t>F806 02CB</t>
   </si>
   <si>
-    <t>B5FF FF6B</t>
-  </si>
-  <si>
-    <t>B500 0109</t>
-  </si>
-  <si>
     <t>1400 0040</t>
   </si>
   <si>
@@ -174,9 +168,6 @@
     <t>11111000000</t>
   </si>
   <si>
-    <t>10110101</t>
-  </si>
-  <si>
     <t>000101</t>
   </si>
   <si>
@@ -247,6 +238,21 @@
   </si>
   <si>
     <t>X11</t>
+  </si>
+  <si>
+    <t>10110100</t>
+  </si>
+  <si>
+    <t>10110100 1111 1111 1111 1111 0110 1011</t>
+  </si>
+  <si>
+    <t>B4FF FF6B</t>
+  </si>
+  <si>
+    <t>10110100 0000 0000 0000 0001 0000 1001</t>
+  </si>
+  <si>
+    <t>B400 0109</t>
   </si>
 </sst>
 </file>
@@ -616,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,22 +729,22 @@
         <v>38</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -746,34 +752,34 @@
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -781,34 +787,34 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -816,34 +822,34 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -851,34 +857,34 @@
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -886,34 +892,34 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -921,34 +927,34 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -956,69 +962,69 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1026,34 +1032,34 @@
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1061,34 +1067,34 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1096,34 +1102,34 @@
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1131,34 +1137,34 @@
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1166,34 +1172,34 @@
         <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1201,270 +1207,280 @@
         <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G27" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled in ER and ran sim
First try - fail
</commit_message>
<xml_diff>
--- a/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
+++ b/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese\Documents\GitHub\ARM-Lab\ARM-Lab\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese_ford1\Documents\GitHub\ARM-Lab\ARM-Lab\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71793BAC-C5A7-4F50-94F3-603A231BF877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B2C47C-62BE-4EE6-81A8-A4258BE9F84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7260" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="90">
   <si>
     <t>Instruction 1</t>
   </si>
@@ -247,6 +247,54 @@
   </si>
   <si>
     <t>B400 0109</t>
+  </si>
+  <si>
+    <t>cur_pc</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>alu_result (dec)</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>branch_target (dec)</t>
+  </si>
+  <si>
+    <t>zero (bin)</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>-192</t>
   </si>
 </sst>
 </file>
@@ -328,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -336,6 +384,8 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,187 +721,187 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>31</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>72</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>55</v>
@@ -860,19 +910,19 @@
         <v>55</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>55</v>
@@ -883,7 +933,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>55</v>
@@ -898,16 +948,16 @@
         <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>55</v>
@@ -918,10 +968,10 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>55</v>
@@ -933,10 +983,10 @@
         <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>55</v>
@@ -953,7 +1003,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>56</v>
@@ -965,13 +1015,13 @@
         <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>55</v>
@@ -988,25 +1038,25 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>55</v>
@@ -1015,33 +1065,33 @@
         <v>55</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>55</v>
@@ -1050,18 +1100,18 @@
         <v>55</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>55</v>
@@ -1093,19 +1143,19 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>55</v>
@@ -1120,69 +1170,69 @@
         <v>55</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1190,280 +1240,420 @@
         <v>50</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>59</v>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>55</v>
+        <v>69</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated TC1, TC2, and TC3
</commit_message>
<xml_diff>
--- a/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
+++ b/ARM-Lab/tables/Lab6_ExpectedResultsTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese_ford1\Documents\GitHub\ARM-Lab\ARM-Lab\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE46DEC-5943-475A-A586-8B86126969A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABF0250-B9B6-4090-B38F-C5EC6F6849D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="0" windowWidth="21240" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7185" yWindow="825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -391,8 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,6 +672,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1433,16 +1435,6 @@
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1683,6 +1675,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="48" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>